<commit_message>
edit name of export template
</commit_message>
<xml_diff>
--- a/export/IHR Costing Tool - Detailed Report Template.xlsx
+++ b/export/IHR Costing Tool - Detailed Report Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13032" activeTab="1" xr2:uid="{E1F37E5D-701C-4E0F-9790-B519BA336093}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13032" xr2:uid="{E1F37E5D-701C-4E0F-9790-B519BA336093}"/>
   </bookViews>
   <sheets>
     <sheet name="Costs" sheetId="1" r:id="rId1"/>
@@ -418,6 +418,7 @@
   </si>
   <si>
     <t>This detailed report contains the cost inputs entered by the user in the Costing page of the IHR Costing Tool. Gray rows represent inputs, such as “Hold annual national conference on IHR laboratory plan implementation and coordination”, and show the user-specified total costs for the input in the final two columns. White rows are the detailed, default line item cost calculations for each input, such as “Conference per diems”. The calculations for the line item costs are shown in the multiplier columns.
+The legend below defines the contents of each column and the example walks through how they apply to calculating a specific line item cost.
 In example 1 below, the cost “Conference per diems” includes the daily domestic per diem per person, times 1 annual conference lasting 3 days, times 30 people (105 USD * 1 * 3 * 30). Because this is a recurring line item, the total (9,450 USD) appears in column W, “Annual recurring costs”.
 Note that costs to increase from score 4 to 5 are highly country-specific and are not included in the IHR Costing Tool.</t>
   </si>
@@ -642,13 +643,13 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,7 +966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0BAA1C-8812-4BC1-86BB-AD3EF649F296}">
   <dimension ref="A1:V1500"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -37034,9 +37035,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B62A33A-A79D-4D31-A8E3-5D09AAE70E3B}">
   <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:B1"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37054,7 +37055,7 @@
         <v>72</v>
       </c>
       <c r="B1" s="24"/>
-      <c r="C1" s="25"/>
+      <c r="C1" s="23"/>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
       <c r="F1" s="22"/>
@@ -37067,12 +37068,12 @@
       <c r="M1" s="22"/>
       <c r="N1" s="22"/>
     </row>
-    <row r="2" spans="1:23" ht="202.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:23" ht="244.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
     </row>
     <row r="3" spans="1:23" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">

</xml_diff>

<commit_message>
updat etemplate structure for XLS export
</commit_message>
<xml_diff>
--- a/export/IHR Costing Tool - Detailed Report Template.xlsx
+++ b/export/IHR Costing Tool - Detailed Report Template.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
   <si>
     <t>Line item ID</t>
   </si>
@@ -85,12 +85,6 @@
   </si>
   <si>
     <t>Staff multiplier unit</t>
-  </si>
-  <si>
-    <t>Do not edit: Start-up/Capital costs</t>
-  </si>
-  <si>
-    <t>Do not edit: Annual recurring costs</t>
   </si>
   <si>
     <t>Column name</t>
@@ -1043,10 +1037,10 @@
         <v>19</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -37052,7 +37046,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A1" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="23"/>
@@ -37070,14 +37064,14 @@
     </row>
     <row r="2" spans="1:23" ht="244.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
     </row>
     <row r="3" spans="1:23" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -37140,160 +37134,160 @@
         <v>19</v>
       </c>
       <c r="V3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" s="20" customFormat="1" ht="180" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="S4" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="T4" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="U4" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="V4" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="W4" s="19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="20" customFormat="1" ht="180" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+    <row r="5" spans="1:23" s="16" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>28</v>
+      <c r="D5" s="12" t="s">
+        <v>29</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>30</v>
+      <c r="E5" s="13" t="s">
+        <v>68</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>47</v>
+      <c r="F5" s="13" t="s">
+        <v>68</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>48</v>
+      <c r="G5" s="13" t="s">
+        <v>68</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>49</v>
+      <c r="H5" s="13" t="s">
+        <v>69</v>
       </c>
-      <c r="H4" s="17" t="s">
-        <v>50</v>
+      <c r="I5" s="13" t="s">
+        <v>68</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>51</v>
+      <c r="J5" s="13" t="s">
+        <v>67</v>
       </c>
-      <c r="J4" s="17" t="s">
-        <v>52</v>
+      <c r="K5" s="13" t="s">
+        <v>68</v>
       </c>
-      <c r="K4" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="M4" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="N4" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="O4" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="P4" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q4" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="R4" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="S4" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="T4" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="U4" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="V4" s="19" t="s">
+      <c r="L5" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="W4" s="19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" s="16" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="L5" s="13" t="s">
+      <c r="M5" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="M5" s="13" t="s">
-        <v>70</v>
+      <c r="N5" s="13" t="s">
+        <v>66</v>
       </c>
-      <c r="N5" s="13" t="s">
+      <c r="O5" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="O5" s="13" t="s">
-        <v>70</v>
+      <c r="P5" s="13" t="s">
+        <v>66</v>
       </c>
-      <c r="P5" s="13" t="s">
+      <c r="Q5" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Q5" s="13" t="s">
-        <v>70</v>
+      <c r="R5" s="13" t="s">
+        <v>66</v>
       </c>
-      <c r="R5" s="13" t="s">
+      <c r="S5" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="S5" s="13" t="s">
-        <v>70</v>
+      <c r="T5" s="13" t="s">
+        <v>66</v>
       </c>
-      <c r="T5" s="13" t="s">
+      <c r="U5" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="U5" s="13" t="s">
-        <v>70</v>
-      </c>
       <c r="V5" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="W5" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:23" s="20" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" s="12">
         <v>1</v>
@@ -37302,55 +37296,55 @@
         <v>2</v>
       </c>
       <c r="E6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="H6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="I6" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="J6" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="K6" s="17" t="s">
         <v>37</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>39</v>
       </c>
       <c r="L6" s="14">
         <v>105</v>
       </c>
       <c r="M6" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N6" s="17">
         <v>1</v>
       </c>
       <c r="O6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q6" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="P6" s="17" t="s">
+      <c r="R6" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="Q6" s="17" t="s">
+      <c r="S6" s="17" t="s">
         <v>43</v>
-      </c>
-      <c r="R6" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="S6" s="17" t="s">
-        <v>45</v>
       </c>
       <c r="T6" s="17">
         <v>30</v>
       </c>
       <c r="U6" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="V6" s="19">
         <v>0</v>

</xml_diff>

<commit_message>
update detailed report template per justin suggestions
</commit_message>
<xml_diff>
--- a/export/IHR Costing Tool - Detailed Report Template.xlsx
+++ b/export/IHR Costing Tool - Detailed Report Template.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Costs" sheetId="1" r:id="rId1"/>
     <sheet name="Legend" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
   <si>
     <t>Line item ID</t>
   </si>
   <si>
     <t>Indicator</t>
-  </si>
-  <si>
-    <t>Starting score</t>
   </si>
   <si>
     <t>Action</t>
@@ -97,9 +94,6 @@
   </si>
   <si>
     <t>Unique ID and name of the indicator costed</t>
-  </si>
-  <si>
-    <t>User's starting score for the indicator</t>
   </si>
   <si>
     <t>1, 2, 3, 4, or 5</t>
@@ -408,13 +402,27 @@
     <t>An indicator JEE ID (e.g., P.1.1) followed by its name</t>
   </si>
   <si>
-    <t>User's target score for the indicator. Note that costs to increase from score 4 to 5 are highly country-specific and are not included in the IHR Costing Tool.</t>
-  </si>
-  <si>
     <t>2, 3, or 4</t>
   </si>
   <si>
     <t>Target score</t>
+  </si>
+  <si>
+    <t>Current score 
+(Entered in tool)</t>
+  </si>
+  <si>
+    <t>Target score
+(Chosen in tool)</t>
+  </si>
+  <si>
+    <t>Current score</t>
+  </si>
+  <si>
+    <t>Current  score for the indicator</t>
+  </si>
+  <si>
+    <t>Target score for the indicator. Note that costs to increase from score 4 to 5 are highly country-specific and are not included in the IHR Costing Tool.</t>
   </si>
 </sst>
 </file>
@@ -982,67 +990,67 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="U1" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -37048,7 +37056,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="23"/>
@@ -37066,230 +37074,230 @@
     </row>
     <row r="2" spans="1:23" ht="244.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
     </row>
     <row r="3" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="U3" s="2" t="s">
-        <v>18</v>
+      <c r="V3" s="3" t="s">
+        <v>56</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" s="20" customFormat="1" ht="180" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="S4" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="T4" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="U4" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="V4" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="W4" s="19" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="20" customFormat="1" ht="180" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+    <row r="5" spans="1:23" s="16" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="P5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="R5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="S5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="T5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="U5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="V5" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="W5" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" s="20" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="B6" s="21" t="s">
         <v>24</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="M4" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="N4" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="O4" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="P4" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q4" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="R4" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="S4" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="T4" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="U4" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="V4" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="W4" s="19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" s="16" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="P5" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q5" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="R5" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="S5" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="T5" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="U5" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="V5" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="W5" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" s="20" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>26</v>
       </c>
       <c r="C6" s="12">
         <v>1</v>
@@ -37298,55 +37306,55 @@
         <v>2</v>
       </c>
       <c r="E6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="H6" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="I6" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="J6" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="K6" s="17" t="s">
         <v>31</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>33</v>
       </c>
       <c r="L6" s="14">
         <v>105</v>
       </c>
       <c r="M6" s="18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N6" s="17">
         <v>1</v>
       </c>
       <c r="O6" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="17" t="s">
+      <c r="R6" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="Q6" s="17" t="s">
+      <c r="S6" s="17" t="s">
         <v>37</v>
-      </c>
-      <c r="R6" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="S6" s="17" t="s">
-        <v>39</v>
       </c>
       <c r="T6" s="17">
         <v>30</v>
       </c>
       <c r="U6" s="17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="V6" s="19">
         <v>0</v>

</xml_diff>

<commit_message>
switched flag back -_-
</commit_message>
<xml_diff>
--- a/export/IHR Costing Tool - Detailed Report Template.xlsx
+++ b/export/IHR Costing Tool - Detailed Report Template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,7 @@
     <sheet name="Costs" sheetId="1" r:id="rId1"/>
     <sheet name="Legend" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
   <si>
     <t>Line item ID</t>
   </si>
   <si>
     <t>Indicator</t>
-  </si>
-  <si>
-    <t>Starting score</t>
-  </si>
-  <si>
-    <t>Target Score</t>
   </si>
   <si>
     <t>Action</t>
@@ -87,12 +81,6 @@
     <t>Staff multiplier unit</t>
   </si>
   <si>
-    <t>Do not edit: Start-up/Capital costs</t>
-  </si>
-  <si>
-    <t>Do not edit: Annual recurring costs</t>
-  </si>
-  <si>
     <t>Column name</t>
   </si>
   <si>
@@ -105,22 +93,10 @@
     <t>Valid column values</t>
   </si>
   <si>
-    <t>An indicator JEE ID (e.g., P.1.1) follow by its name</t>
-  </si>
-  <si>
     <t>Unique ID and name of the indicator costed</t>
   </si>
   <si>
-    <t>User's starting score for the indicator</t>
-  </si>
-  <si>
     <t>1, 2, 3, 4, or 5</t>
-  </si>
-  <si>
-    <t>User's target score for the indicator</t>
-  </si>
-  <si>
-    <t>2, 3, 4, or 5</t>
   </si>
   <si>
     <t>D.1.1 Laboratory testing for detection of priority diseases</t>
@@ -413,12 +389,47 @@
 Recurring</t>
     </r>
   </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>This detailed report contains the cost inputs entered by the user in the Costing page of the IHR Costing Tool. Gray rows represent inputs, such as “Hold annual national conference on IHR laboratory plan implementation and coordination”, and show the user-specified total costs for the input in the final two columns. White rows are the detailed, default line item cost calculations for each input, such as “Conference per diems”. The calculations for the line item costs are shown in the multiplier columns.
+The legend below defines the contents of each column and the example walks through how they apply to calculating a specific line item cost.
+In example 1 below, the cost “Conference per diems” includes the daily domestic per diem per person, times 1 annual conference lasting 3 days, times 30 people (105 USD * 1 * 3 * 30). Because this is a recurring line item, the total (9,450 USD) appears in column W, “Annual recurring costs”.
+Note that costs to increase from score 4 to 5 are highly country-specific and are not included in the IHR Costing Tool.</t>
+  </si>
+  <si>
+    <t>An indicator JEE ID (e.g., P.1.1) followed by its name</t>
+  </si>
+  <si>
+    <t>2, 3, or 4</t>
+  </si>
+  <si>
+    <t>Target score</t>
+  </si>
+  <si>
+    <t>Current score 
+(Entered in tool)</t>
+  </si>
+  <si>
+    <t>Target score
+(Chosen in tool)</t>
+  </si>
+  <si>
+    <t>Current score</t>
+  </si>
+  <si>
+    <t>Current  score for the indicator</t>
+  </si>
+  <si>
+    <t>Target score for the indicator. Note that costs to increase from score 4 to 5 are highly country-specific and are not included in the IHR Costing Tool.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,8 +483,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -510,8 +536,14 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -534,11 +566,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -601,6 +642,14 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -927,7 +976,9 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.140625" customWidth="1"/>
-    <col min="2" max="7" width="25.7109375" customWidth="1"/>
+    <col min="2" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="5" width="38.7109375" customWidth="1"/>
+    <col min="6" max="7" width="25.7109375" customWidth="1"/>
     <col min="8" max="8" width="49.5703125" customWidth="1"/>
     <col min="9" max="9" width="24.7109375" customWidth="1"/>
     <col min="10" max="20" width="25.7109375" customWidth="1"/>
@@ -939,67 +990,67 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="U1" s="3" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -36986,14 +37037,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B62A33A-A79D-4D31-A8E3-5D09AAE70E3B}">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" style="11" customWidth="1"/>
     <col min="2" max="7" width="38.7109375" style="11" customWidth="1"/>
@@ -37003,291 +37054,320 @@
     <col min="24" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:23" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+    </row>
+    <row r="2" spans="1:23" ht="244.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+    </row>
+    <row r="3" spans="1:23" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" s="20" customFormat="1" ht="180" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C4" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="S4" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="T4" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="U4" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="V4" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="W4" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" s="16" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="P5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="R5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="S5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="T5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="U5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="V5" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="W5" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" s="20" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="12">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D6" s="12">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+      <c r="E6" s="12" t="s">
+        <v>25</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+      <c r="F6" s="12" t="s">
+        <v>26</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+      <c r="G6" s="17" t="s">
+        <v>27</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
+      <c r="H6" s="17" t="s">
+        <v>28</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
+      <c r="I6" s="17" t="s">
+        <v>29</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
+      <c r="J6" s="17" t="s">
+        <v>30</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K6" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="14">
+        <v>105</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="17">
+        <v>1</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="T6" s="17">
+        <v>30</v>
+      </c>
+      <c r="U6" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="V6" s="19">
         <v>0</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" s="20" customFormat="1" ht="180" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="O2" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q2" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="R2" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="S2" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="T2" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="U2" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="V2" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="W2" s="19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" s="16" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="R3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="T3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="U3" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="V3" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="W3" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" s="20" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="12">
-        <v>1</v>
-      </c>
-      <c r="D4" s="12">
-        <v>2</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="14">
-        <v>105</v>
-      </c>
-      <c r="M4" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="17">
-        <v>1</v>
-      </c>
-      <c r="O4" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="P4" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q4" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="R4" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="S4" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="T4" s="17">
-        <v>30</v>
-      </c>
-      <c r="U4" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="V4" s="19">
-        <v>0</v>
-      </c>
-      <c r="W4" s="19">
+      <c r="W6" s="19">
         <v>9450</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>